<commit_message>
update % DC in E2b
</commit_message>
<xml_diff>
--- a/Experiment 2b/participant_info.xlsx
+++ b/Experiment 2b/participant_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\preview_costs\Experiment 2b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4846BBD6-FCDC-4112-A656-0A3E36F43444}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85BE46D-EBF9-4EB0-9F7D-8D44F97BBA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,10 +66,10 @@
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
-    awarenes of letter mask degraded changes</t>
+    awarenes of letter mask changes</t>
       </text>
     </comment>
-    <comment ref="G1" authorId="3" shapeId="0" xr:uid="{33F42817-DAE6-4A28-BBFC-8A7AD403C24D}">
+    <comment ref="H1" authorId="3" shapeId="0" xr:uid="{33F42817-DAE6-4A28-BBFC-8A7AD403C24D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -77,7 +77,7 @@
     Percentage of trials with degraded changes</t>
       </text>
     </comment>
-    <comment ref="H1" authorId="4" shapeId="0" xr:uid="{90B15B28-2376-4996-84E4-574011696A06}">
+    <comment ref="I1" authorId="4" shapeId="0" xr:uid="{90B15B28-2376-4996-84E4-574011696A06}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>10 male</t>
+  </si>
+  <si>
+    <t>DC_lett</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,13 +225,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,12 +530,12 @@
     <text>Awareness of orthographical display changes</text>
   </threadedComment>
   <threadedComment ref="F1" dT="2020-02-21T18:49:50.64" personId="{6E0C14D4-C5FB-4AC0-BF98-9D1C137B0F90}" id="{82B20F82-BD10-490C-A1AF-2F9484E604F1}">
-    <text>awarenes of letter mask degraded changes</text>
+    <text>awarenes of letter mask changes</text>
   </threadedComment>
-  <threadedComment ref="G1" dT="2020-02-21T18:51:25.78" personId="{6E0C14D4-C5FB-4AC0-BF98-9D1C137B0F90}" id="{33F42817-DAE6-4A28-BBFC-8A7AD403C24D}">
+  <threadedComment ref="H1" dT="2020-02-21T18:51:25.78" personId="{6E0C14D4-C5FB-4AC0-BF98-9D1C137B0F90}" id="{33F42817-DAE6-4A28-BBFC-8A7AD403C24D}">
     <text>Percentage of trials with degraded changes</text>
   </threadedComment>
-  <threadedComment ref="H1" dT="2020-02-21T18:51:44.20" personId="{6E0C14D4-C5FB-4AC0-BF98-9D1C137B0F90}" id="{90B15B28-2376-4996-84E4-574011696A06}">
+  <threadedComment ref="I1" dT="2020-02-21T18:51:44.20" personId="{6E0C14D4-C5FB-4AC0-BF98-9D1C137B0F90}" id="{90B15B28-2376-4996-84E4-574011696A06}">
     <text>Percentage of trials with orthographical changes</text>
   </threadedComment>
 </ThreadedComments>
@@ -537,21 +543,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="8" width="11.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,16 +578,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -599,16 +609,19 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
         <v>40</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <f>2/138</f>
         <v>1.4492753623188406E-2</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -627,11 +640,14 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -650,11 +666,14 @@
       <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -673,14 +692,17 @@
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -699,11 +721,14 @@
       <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -722,11 +747,14 @@
       <c r="F7" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -745,11 +773,14 @@
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -768,11 +799,14 @@
       <c r="F9" s="2">
         <v>0</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -791,15 +825,18 @@
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
         <v>60</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="9">
         <v>30</v>
       </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -818,11 +855,14 @@
       <c r="F11" s="2">
         <v>0</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -841,13 +881,16 @@
       <c r="F12" s="2">
         <v>0</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
         <v>20</v>
       </c>
-      <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -866,13 +909,16 @@
       <c r="F13" s="2">
         <v>0</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
         <v>60</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -891,17 +937,20 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
         <v>30</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>20</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -920,11 +969,14 @@
       <c r="F15" s="2">
         <v>0</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -943,10 +995,13 @@
       <c r="F16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
       <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -965,11 +1020,14 @@
       <c r="F17" s="2">
         <v>0</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -988,14 +1046,17 @@
       <c r="F18" s="2">
         <v>0</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
         <v>60</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1014,11 +1075,14 @@
       <c r="F19" s="2">
         <v>0</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1037,17 +1101,20 @@
       <c r="F20" s="2">
         <v>1</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
         <v>50</v>
-      </c>
-      <c r="H20" s="3">
-        <v>25</v>
       </c>
       <c r="I20" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1066,14 +1133,17 @@
       <c r="F21" s="2">
         <v>0</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
         <v>40</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1092,14 +1162,17 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
         <v>50</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1118,11 +1191,14 @@
       <c r="F23" s="2">
         <v>0</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1141,11 +1217,14 @@
       <c r="F24" s="2">
         <v>0</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1164,19 +1243,22 @@
       <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
         <v>40</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <f>5/138</f>
         <v>3.6231884057971016E-2</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <f>3/138</f>
         <v>2.1739130434782608E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1195,17 +1277,20 @@
       <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
         <v>40</v>
-      </c>
-      <c r="H26" s="2">
-        <v>20</v>
       </c>
       <c r="I26" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1224,11 +1309,14 @@
       <c r="F27" s="2">
         <v>0</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1247,19 +1335,22 @@
       <c r="F28" s="2">
         <v>1</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
         <v>65</v>
-      </c>
-      <c r="H28" s="2">
-        <f>2/138</f>
-        <v>1.4492753623188406E-2</v>
       </c>
       <c r="I28" s="2">
         <f>2/138</f>
         <v>1.4492753623188406E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="2">
+        <f>2/138</f>
+        <v>1.4492753623188406E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1278,14 +1369,17 @@
       <c r="F29" s="2">
         <v>0</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
         <v>65</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1304,17 +1398,20 @@
       <c r="F30" s="2">
         <v>1</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
         <v>60</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>45</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1333,17 +1430,20 @@
       <c r="F31" s="2">
         <v>1</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="6">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
         <v>65</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>40</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1362,13 +1462,16 @@
       <c r="F32" s="2">
         <v>0</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
         <v>60</v>
       </c>
-      <c r="H32" s="4"/>
       <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1387,11 +1490,14 @@
       <c r="F33" s="2">
         <v>0</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1410,14 +1516,17 @@
       <c r="F34" s="2">
         <v>1</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
         <v>30</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1436,14 +1545,17 @@
       <c r="F35" s="2">
         <v>0</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2">
         <v>40</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1462,14 +1574,17 @@
       <c r="F36" s="2">
         <v>0</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
         <v>17.5</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1488,8 +1603,11 @@
       <c r="F37" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1508,18 +1626,21 @@
       <c r="F38" s="2">
         <v>1</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="6">
+        <v>1</v>
+      </c>
+      <c r="H38" s="2">
         <v>35</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>15</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <f>2/138</f>
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1538,15 +1659,18 @@
       <c r="F39" s="2">
         <v>0</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+      <c r="H39" s="2">
         <v>50</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <f>2/138</f>
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1565,17 +1689,20 @@
       <c r="F40" s="2">
         <v>1</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="6">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
         <v>55</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>35</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1594,17 +1721,20 @@
       <c r="F41" s="2">
         <v>0</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2">
         <v>40</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>70</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1623,14 +1753,17 @@
       <c r="F42" s="2">
         <v>0</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="6">
+        <v>1</v>
+      </c>
+      <c r="H42" s="2">
         <v>40</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1649,14 +1782,17 @@
       <c r="F43" s="2">
         <v>0</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
         <v>50</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1675,17 +1811,20 @@
       <c r="F44" s="2">
         <v>1</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+      <c r="H44" s="2">
         <v>60</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>30</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1704,11 +1843,14 @@
       <c r="F45" s="2">
         <v>0</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="6">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1727,14 +1869,17 @@
       <c r="F46" s="2">
         <v>0</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+      <c r="H46" s="2">
         <v>30</v>
       </c>
-      <c r="H46" s="2">
+      <c r="I46" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1753,18 +1898,21 @@
       <c r="F47" s="2">
         <v>1</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="6">
+        <v>1</v>
+      </c>
+      <c r="H47" s="2">
         <v>60</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>20</v>
       </c>
-      <c r="I47" s="2">
+      <c r="J47" s="2">
         <f>2/138</f>
         <v>1.4492753623188406E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1783,11 +1931,14 @@
       <c r="F48" s="2">
         <v>0</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="6">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1806,11 +1957,14 @@
       <c r="F49" s="2">
         <v>0</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="6">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1829,11 +1983,14 @@
       <c r="F50" s="2">
         <v>0</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="6">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1852,11 +2009,14 @@
       <c r="F51" s="2">
         <v>0</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="6">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1875,11 +2035,14 @@
       <c r="F52" s="2">
         <v>0</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="6">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -1898,13 +2061,16 @@
       <c r="F53" s="2">
         <v>0</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="6">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
         <v>10</v>
       </c>
-      <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -1923,14 +2089,17 @@
       <c r="F54" s="2">
         <v>1</v>
       </c>
-      <c r="H54" s="2">
+      <c r="G54" s="6">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2">
         <v>50</v>
       </c>
-      <c r="I54" s="2">
+      <c r="J54" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -1949,11 +2118,14 @@
       <c r="F55" s="2">
         <v>0</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="H55" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -1972,11 +2144,14 @@
       <c r="F56" s="2">
         <v>0</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="6">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -1995,13 +2170,16 @@
       <c r="F57" s="2">
         <v>0</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="6">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
         <v>40</v>
       </c>
-      <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J57" s="4"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2020,8 +2198,11 @@
       <c r="F58" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2040,11 +2221,14 @@
       <c r="F59" s="2">
         <v>0</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="6">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2063,19 +2247,22 @@
       <c r="F60" s="2">
         <v>1</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="6">
+        <v>1</v>
+      </c>
+      <c r="H60" s="2">
         <v>70</v>
       </c>
-      <c r="H60" s="2">
+      <c r="I60" s="2">
         <f>3/138</f>
         <v>2.1739130434782608E-2</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <f>1/138</f>
         <v>7.246376811594203E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2094,13 +2281,16 @@
       <c r="F61" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G61" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>11</v>
       </c>
@@ -2108,8 +2298,16 @@
         <f>AVERAGE(C2:C61)</f>
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D63" s="2">
+        <f>SUM(D2:D61)/60</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="G63" s="6">
+        <f>SUM(G2:G61)/60</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>12</v>
       </c>
@@ -2138,9 +2336,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>